<commit_message>
sending confirmation email is done and is integrated into post reservation via background task, reworked csv sessions uploading
</commit_message>
<xml_diff>
--- a/fastapi/csv_examples/session.xlsx
+++ b/fastapi/csv_examples/session.xlsx
@@ -20,11 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Дата и время</t>
   </si>
   <si>
+    <t xml:space="preserve">Бронь закрыта</t>
+  </si>
+  <si>
     <t xml:space="preserve">id спектакль</t>
   </si>
   <si>
@@ -34,7 +37,13 @@
     <t xml:space="preserve">07-02-2022 10:30</t>
   </si>
   <si>
+    <t xml:space="preserve">Д</t>
+  </si>
+  <si>
     <t xml:space="preserve">07-02-2022 14:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Н</t>
   </si>
 </sst>
 </file>
@@ -49,6 +58,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -130,13 +140,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
@@ -153,26 +163,35 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>7</v>
       </c>
       <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>